<commit_message>
debug temporal dynamic analyzer
</commit_message>
<xml_diff>
--- a/sim11.1_moreClasses342/PROTO3.xlsx
+++ b/sim11.1_moreClasses342/PROTO3.xlsx
@@ -20,7 +20,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -31,6 +31,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -53,14 +69,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -390,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ9"/>
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -423,109 +447,109 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AF2">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AG2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AH2">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AJ2">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -590,16 +614,16 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <v>0</v>
@@ -651,29 +675,29 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1</v>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -706,16 +730,16 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4">
         <v>0</v>
@@ -822,16 +846,16 @@
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -883,29 +907,29 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1</v>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -938,16 +962,16 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -1054,16 +1078,16 @@
         <v>0</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7">
         <v>0</v>
@@ -1115,29 +1139,29 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>1</v>
-      </c>
-      <c r="R8" s="1">
-        <v>1</v>
-      </c>
-      <c r="S8" s="1">
-        <v>1</v>
-      </c>
-      <c r="T8" s="1">
-        <v>1</v>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1170,16 +1194,16 @@
         <v>0</v>
       </c>
       <c r="AE8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -1286,20 +1310,131 @@
         <v>0</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
+        <v>1</v>
+      </c>
+      <c r="T10" s="1">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>